<commit_message>
Create gull population distribution graph
</commit_message>
<xml_diff>
--- a/data/gull_pop_distribution_2022.xlsx
+++ b/data/gull_pop_distribution_2022.xlsx
@@ -1,25 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janderson\Desktop\addisons archive\gdi_master\data\bird\gulls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wrileyhodge/Wriley and Eleanor Final Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2B332F-3727-9C49-AC65-6AB7B2327B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="COA_Property">Sheet1!$O$1</definedName>
     <definedName name="total_TNC_IFW" localSheetId="0">Sheet1!$Q$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -105,7 +118,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -162,6 +175,227 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.2182852143482065E-2"/>
+          <c:y val="7.4548702245552642E-2"/>
+          <c:w val="0.73812357830271214"/>
+          <c:h val="0.8326195683872849"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Borofsky Inholding</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2015</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$3:$H$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>262</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DABF-4C50-A769-0458CE365C9C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="128877696"/>
+        <c:axId val="76808960"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="128877696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="76808960"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="76808960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="128877696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
       <c14:style val="118"/>
     </mc:Choice>
     <mc:Fallback>
@@ -186,7 +420,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -364,7 +597,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-80CF-40C2-965E-84BBB3BDE96B}"/>
+              <c16:uniqueId val="{00000000-C836-2C4E-B98A-EFE2BA3EAE26}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -536,7 +769,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-80CF-40C2-965E-84BBB3BDE96B}"/>
+              <c16:uniqueId val="{00000001-C836-2C4E-B98A-EFE2BA3EAE26}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -599,7 +832,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -623,7 +855,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -658,7 +890,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -836,7 +1067,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7BCB-45A7-A1AC-1AD5338C0D64}"/>
+              <c16:uniqueId val="{00000000-401B-6A45-A1D4-B1CA46945A6D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -899,7 +1130,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
@@ -923,302 +1153,8 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="7.2182852143482065E-2"/>
-          <c:y val="7.4548702245552642E-2"/>
-          <c:w val="0.73812357830271214"/>
-          <c:h val="0.8326195683872849"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Borofsky Inholding</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$3:$A$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2004</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2005</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2006</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2007</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2008</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2009</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2010</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2011</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2012</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2013</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2015</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$H$3:$H$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>105</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>125</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>116</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>113</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>123</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>183</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>149</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>262</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>152</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>162</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>109</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>72</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-DABF-4C50-A769-0458CE365C9C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="128877696"/>
-        <c:axId val="76808960"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="128877696"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76808960"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="76808960"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128877696"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>147320</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>690562</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>119063</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>354013</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>59531</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
@@ -1249,7 +1185,88 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>147320</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>690562</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{095970D6-976C-6D4D-86C9-827B3FA022BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>354013</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>59531</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F8A4964-099A-A348-8D07-8037797AF949}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1579,16 +1596,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="K57" sqref="K57"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1638,7 +1655,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1999</v>
       </c>
@@ -1685,7 +1702,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2000</v>
       </c>
@@ -1735,7 +1752,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2001</v>
       </c>
@@ -1780,7 +1797,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2002</v>
       </c>
@@ -1829,7 +1846,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2003</v>
       </c>
@@ -1872,7 +1889,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2004</v>
       </c>
@@ -1924,7 +1941,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2005</v>
       </c>
@@ -1976,7 +1993,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2006</v>
       </c>
@@ -2028,7 +2045,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2007</v>
       </c>
@@ -2077,7 +2094,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2008</v>
       </c>
@@ -2129,7 +2146,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2009</v>
       </c>
@@ -2181,7 +2198,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2010</v>
       </c>
@@ -2207,7 +2224,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2011</v>
       </c>
@@ -2256,7 +2273,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2012</v>
       </c>
@@ -2304,7 +2321,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2013</v>
       </c>
@@ -2353,7 +2370,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2014</v>
       </c>
@@ -2398,7 +2415,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2015</v>
       </c>
@@ -2443,7 +2460,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2016</v>
       </c>
@@ -2488,7 +2505,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2017</v>
       </c>
@@ -2533,7 +2550,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2018</v>
       </c>
@@ -2578,7 +2595,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2019</v>
       </c>
@@ -2617,7 +2634,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2020</v>
       </c>
@@ -2662,7 +2679,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2021</v>
       </c>
@@ -2707,7 +2724,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.6">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2022</v>
       </c>
@@ -2750,37 +2767,6 @@
       <c r="Q25">
         <f t="shared" si="1"/>
         <v>328</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.6">
-      <c r="A26" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.6">
-      <c r="A28" t="s">
-        <v>18</v>
-      </c>
-      <c r="G28" t="s">
-        <v>23</v>
-      </c>
-      <c r="I28" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.6">
-      <c r="A29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.6">
-      <c r="A30" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.6">
-      <c r="A31" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -2792,4 +2778,51 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{102C874C-5A90-524D-AE09-DB95DB1F6978}">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Clean nest count 2021 and 2022
</commit_message>
<xml_diff>
--- a/data/gull_pop_distribution_2022.xlsx
+++ b/data/gull_pop_distribution_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wrileyhodge/Wriley and Eleanor Final Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2B332F-3727-9C49-AC65-6AB7B2327B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64AFFA2B-73DD-124E-8E23-98370A4B8E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <definedName name="COA_Property">Sheet1!$O$1</definedName>
     <definedName name="total_TNC_IFW" localSheetId="0">Sheet1!$Q$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1600,7 +1600,7 @@
   <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>